<commit_message>
Ajout de 3 partenaires en plus et coche si projet terminé
</commit_message>
<xml_diff>
--- a/src/main/resources/weamec/excel_template.xlsx
+++ b/src/main/resources/weamec/excel_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="1" windowWidth="14400" windowHeight="6140"/>
+    <workbookView activeTab="0" windowWidth="19100" windowHeight="8130"/>
   </bookViews>
   <sheets>
     <sheet name="Infos projets" sheetId="1" r:id="rId1"/>
@@ -22,12 +22,84 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2" count="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26" count="26">
+  <si>
+    <t>Partenaires</t>
+  </si>
+  <si>
+    <t>Partenaire 1</t>
+  </si>
+  <si>
+    <t>Partenaire 2</t>
+  </si>
+  <si>
+    <t>Partenaire 3</t>
+  </si>
   <si>
     <t>Brevet</t>
   </si>
   <si>
-    <t>EXPERTS</t>
+    <t>Partenaire 1 : Etalissement ou entreprise</t>
+  </si>
+  <si>
+    <t>Partenaire 1 : code postal</t>
+  </si>
+  <si>
+    <t>Partenaire 1 : ville</t>
+  </si>
+  <si>
+    <t>Partenaire 1 : Laboratoire (si renseigné)</t>
+  </si>
+  <si>
+    <t>Partenaire 1 : Nom </t>
+  </si>
+  <si>
+    <t>Partenaire 1 : Prénom</t>
+  </si>
+  <si>
+    <t>Partenaire 1 : adresse mail</t>
+  </si>
+  <si>
+    <t>Partenaire 2 : Etalissement ou entreprise</t>
+  </si>
+  <si>
+    <t>Partenaire 2 : code postal</t>
+  </si>
+  <si>
+    <t>Partenaire 2 : ville</t>
+  </si>
+  <si>
+    <t>Partenaire 2 : Laboratoire (si renseigné)</t>
+  </si>
+  <si>
+    <t>Partenaire 2 : Nom </t>
+  </si>
+  <si>
+    <t>Partenaire 2 : Prénom</t>
+  </si>
+  <si>
+    <t>Partenaire 2 : adresse mail</t>
+  </si>
+  <si>
+    <t>Partenaire 3 : Etalissement ou entreprise</t>
+  </si>
+  <si>
+    <t>Partenaire 3 : code postal</t>
+  </si>
+  <si>
+    <t>Partenaire 3 : ville</t>
+  </si>
+  <si>
+    <t>Partenaire 3 : Laboratoire (si renseigné)</t>
+  </si>
+  <si>
+    <t>Partenaire 3 : Nom </t>
+  </si>
+  <si>
+    <t>Partenaire 3 : Prénom</t>
+  </si>
+  <si>
+    <t>Partenaire 3 : adresse mail</t>
   </si>
 </sst>
 </file>
@@ -624,10 +696,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:CX3"/>
+  <dimension ref="A1:DS3"/>
   <sheetViews>
-    <sheetView topLeftCell="CI1" workbookViewId="0" zoomScale="60">
-      <selection activeCell="CX3" sqref="A1:CX3"/>
+    <sheetView topLeftCell="AE1" workbookViewId="0" tabSelected="1">
+      <selection activeCell="AM19" sqref="AM19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="67.5" defaultRowHeight="14.4"/>
@@ -635,7 +707,7 @@
     <col min="1" max="16384" style="1" width="12.856370192307693"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:102" ht="15">
+    <row r="1" spans="1:123" ht="15">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="inlineStr">
         <is>
@@ -649,10 +721,8 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="4"/>
-      <c r="J1" s="5" t="inlineStr">
-        <is>
-          <t>Partenaires</t>
-        </is>
+      <c r="J1" s="5" t="s">
+        <v>0</v>
       </c>
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
@@ -680,49 +750,49 @@
       <c r="AH1" s="6"/>
       <c r="AI1" s="6"/>
       <c r="AJ1" s="7"/>
-      <c r="AK1" s="8" t="inlineStr">
+      <c r="AK1" s="7"/>
+      <c r="AL1" s="7"/>
+      <c r="AM1" s="7"/>
+      <c r="AN1" s="7"/>
+      <c r="AO1" s="7"/>
+      <c r="AP1" s="7"/>
+      <c r="AQ1" s="7"/>
+      <c r="AR1" s="7"/>
+      <c r="AS1" s="7"/>
+      <c r="AT1" s="7"/>
+      <c r="AU1" s="7"/>
+      <c r="AV1" s="7"/>
+      <c r="AW1" s="7"/>
+      <c r="AX1" s="7"/>
+      <c r="AY1" s="7"/>
+      <c r="AZ1" s="7"/>
+      <c r="BA1" s="7"/>
+      <c r="BB1" s="7"/>
+      <c r="BC1" s="7"/>
+      <c r="BD1" s="7"/>
+      <c r="BE1" s="7"/>
+      <c r="BF1" s="8" t="inlineStr">
         <is>
           <t>Finances et RH</t>
         </is>
       </c>
-      <c r="AL1" s="9"/>
-      <c r="AM1" s="9"/>
-      <c r="AN1" s="9"/>
-      <c r="AO1" s="9"/>
-      <c r="AP1" s="9"/>
-      <c r="AQ1" s="9"/>
-      <c r="AR1" s="9"/>
-      <c r="AS1" s="9"/>
-      <c r="AT1" s="9"/>
-      <c r="AU1" s="9"/>
-      <c r="AV1" s="9"/>
-      <c r="AW1" s="10"/>
-      <c r="AX1" s="11" t="inlineStr">
+      <c r="BG1" s="9"/>
+      <c r="BH1" s="9"/>
+      <c r="BI1" s="9"/>
+      <c r="BJ1" s="9"/>
+      <c r="BK1" s="9"/>
+      <c r="BL1" s="9"/>
+      <c r="BM1" s="9"/>
+      <c r="BN1" s="9"/>
+      <c r="BO1" s="9"/>
+      <c r="BP1" s="9"/>
+      <c r="BQ1" s="9"/>
+      <c r="BR1" s="10"/>
+      <c r="BS1" s="11" t="inlineStr">
         <is>
           <t>Catégories</t>
         </is>
       </c>
-      <c r="AY1" s="12"/>
-      <c r="AZ1" s="12"/>
-      <c r="BA1" s="12"/>
-      <c r="BB1" s="12"/>
-      <c r="BC1" s="12"/>
-      <c r="BD1" s="12"/>
-      <c r="BE1" s="12"/>
-      <c r="BF1" s="12"/>
-      <c r="BG1" s="12"/>
-      <c r="BH1" s="12"/>
-      <c r="BI1" s="12"/>
-      <c r="BJ1" s="12"/>
-      <c r="BK1" s="12"/>
-      <c r="BL1" s="12"/>
-      <c r="BM1" s="12"/>
-      <c r="BN1" s="12"/>
-      <c r="BO1" s="12"/>
-      <c r="BP1" s="12"/>
-      <c r="BQ1" s="12"/>
-      <c r="BR1" s="12"/>
-      <c r="BS1" s="12"/>
       <c r="BT1" s="12"/>
       <c r="BU1" s="12"/>
       <c r="BV1" s="12"/>
@@ -738,32 +808,53 @@
       <c r="CF1" s="12"/>
       <c r="CG1" s="12"/>
       <c r="CH1" s="12"/>
-      <c r="CI1" s="13"/>
-      <c r="CJ1" s="14" t="inlineStr">
+      <c r="CI1" s="12"/>
+      <c r="CJ1" s="12"/>
+      <c r="CK1" s="12"/>
+      <c r="CL1" s="12"/>
+      <c r="CM1" s="12"/>
+      <c r="CN1" s="12"/>
+      <c r="CO1" s="12"/>
+      <c r="CP1" s="12"/>
+      <c r="CQ1" s="12"/>
+      <c r="CR1" s="12"/>
+      <c r="CS1" s="12"/>
+      <c r="CT1" s="12"/>
+      <c r="CU1" s="12"/>
+      <c r="CV1" s="12"/>
+      <c r="CW1" s="12"/>
+      <c r="CX1" s="12"/>
+      <c r="CY1" s="12"/>
+      <c r="CZ1" s="12"/>
+      <c r="DA1" s="12"/>
+      <c r="DB1" s="12"/>
+      <c r="DC1" s="12"/>
+      <c r="DD1" s="13"/>
+      <c r="DE1" s="14" t="inlineStr">
         <is>
           <t>Valorisation du projet</t>
         </is>
       </c>
-      <c r="CK1" s="15"/>
-      <c r="CL1" s="15"/>
-      <c r="CM1" s="15"/>
-      <c r="CN1" s="15"/>
-      <c r="CO1" s="15"/>
-      <c r="CP1" s="15"/>
-      <c r="CQ1" s="15"/>
-      <c r="CR1" s="15"/>
-      <c r="CS1" s="15"/>
-      <c r="CT1" s="15"/>
-      <c r="CU1" s="15"/>
-      <c r="CV1" s="15"/>
-      <c r="CW1" s="16"/>
-      <c r="CX1" s="17" t="inlineStr">
+      <c r="DF1" s="15"/>
+      <c r="DG1" s="15"/>
+      <c r="DH1" s="15"/>
+      <c r="DI1" s="15"/>
+      <c r="DJ1" s="15"/>
+      <c r="DK1" s="15"/>
+      <c r="DL1" s="15"/>
+      <c r="DM1" s="15"/>
+      <c r="DN1" s="15"/>
+      <c r="DO1" s="15"/>
+      <c r="DP1" s="15"/>
+      <c r="DQ1" s="15"/>
+      <c r="DR1" s="16"/>
+      <c r="DS1" s="17" t="inlineStr">
         <is>
           <t>Fin</t>
         </is>
       </c>
     </row>
-    <row r="2" spans="1:102" ht="16.2">
+    <row r="2" spans="1:123" ht="16.2">
       <c r="A2" s="18"/>
       <c r="B2" s="19" t="inlineStr">
         <is>
@@ -795,10 +886,8 @@
       <c r="M2" s="24"/>
       <c r="N2" s="24"/>
       <c r="O2" s="25"/>
-      <c r="P2" s="26" t="inlineStr">
-        <is>
-          <t>Partenaire 1</t>
-        </is>
+      <c r="P2" s="26" t="s">
+        <v>1</v>
       </c>
       <c r="Q2" s="27"/>
       <c r="R2" s="27"/>
@@ -806,10 +895,8 @@
       <c r="T2" s="27"/>
       <c r="U2" s="27"/>
       <c r="V2" s="28"/>
-      <c r="W2" s="26" t="inlineStr">
-        <is>
-          <t>Partenaire 2</t>
-        </is>
+      <c r="W2" s="26" t="s">
+        <v>2</v>
       </c>
       <c r="X2" s="27"/>
       <c r="Y2" s="27"/>
@@ -817,10 +904,8 @@
       <c r="AA2" s="27"/>
       <c r="AB2" s="27"/>
       <c r="AC2" s="28"/>
-      <c r="AD2" s="26" t="inlineStr">
-        <is>
-          <t>Partenaire 3</t>
-        </is>
+      <c r="AD2" s="26" t="s">
+        <v>3</v>
       </c>
       <c r="AE2" s="27"/>
       <c r="AF2" s="27"/>
@@ -828,118 +913,151 @@
       <c r="AH2" s="27"/>
       <c r="AI2" s="27"/>
       <c r="AJ2" s="28"/>
-      <c r="AK2" s="29" t="inlineStr">
+      <c r="AK2" s="26" t="inlineStr">
+        <is>
+          <t>Partenaire 4</t>
+        </is>
+      </c>
+      <c r="AL2" s="27"/>
+      <c r="AM2" s="27"/>
+      <c r="AN2" s="27"/>
+      <c r="AO2" s="27"/>
+      <c r="AP2" s="27"/>
+      <c r="AQ2" s="28"/>
+      <c r="AR2" s="26" t="inlineStr">
+        <is>
+          <t>Partenaire 5</t>
+        </is>
+      </c>
+      <c r="AS2" s="27"/>
+      <c r="AT2" s="27"/>
+      <c r="AU2" s="27"/>
+      <c r="AV2" s="27"/>
+      <c r="AW2" s="27"/>
+      <c r="AX2" s="28"/>
+      <c r="AY2" s="26" t="inlineStr">
+        <is>
+          <t>Partenaire 6</t>
+        </is>
+      </c>
+      <c r="AZ2" s="27"/>
+      <c r="BA2" s="27"/>
+      <c r="BB2" s="27"/>
+      <c r="BC2" s="27"/>
+      <c r="BD2" s="27"/>
+      <c r="BE2" s="28"/>
+      <c r="BF2" s="29" t="inlineStr">
         <is>
           <t>Financement</t>
         </is>
       </c>
-      <c r="AL2" s="30"/>
-      <c r="AM2" s="30"/>
-      <c r="AN2" s="30"/>
-      <c r="AO2" s="30"/>
-      <c r="AP2" s="30"/>
-      <c r="AQ2" s="30"/>
-      <c r="AR2" s="30"/>
-      <c r="AS2" s="30"/>
-      <c r="AT2" s="30"/>
-      <c r="AU2" s="31"/>
-      <c r="AV2" s="29" t="inlineStr">
+      <c r="BG2" s="30"/>
+      <c r="BH2" s="30"/>
+      <c r="BI2" s="30"/>
+      <c r="BJ2" s="30"/>
+      <c r="BK2" s="30"/>
+      <c r="BL2" s="30"/>
+      <c r="BM2" s="30"/>
+      <c r="BN2" s="30"/>
+      <c r="BO2" s="30"/>
+      <c r="BP2" s="31"/>
+      <c r="BQ2" s="29" t="inlineStr">
         <is>
           <t>RH</t>
         </is>
       </c>
-      <c r="AW2" s="31"/>
-      <c r="AX2" s="32" t="inlineStr">
+      <c r="BR2" s="31"/>
+      <c r="BS2" s="32" t="inlineStr">
         <is>
           <t>Technologie (si "Toutes EMR", cocher toutes les cases)</t>
         </is>
       </c>
-      <c r="AY2" s="33"/>
-      <c r="AZ2" s="33"/>
-      <c r="BA2" s="33"/>
-      <c r="BB2" s="33"/>
-      <c r="BC2" s="33"/>
-      <c r="BD2" s="34"/>
-      <c r="BE2" s="32" t="inlineStr">
+      <c r="BT2" s="33"/>
+      <c r="BU2" s="33"/>
+      <c r="BV2" s="33"/>
+      <c r="BW2" s="33"/>
+      <c r="BX2" s="33"/>
+      <c r="BY2" s="34"/>
+      <c r="BZ2" s="32" t="inlineStr">
         <is>
           <t>Thématique</t>
         </is>
       </c>
-      <c r="BF2" s="33"/>
-      <c r="BG2" s="33"/>
-      <c r="BH2" s="33"/>
-      <c r="BI2" s="34"/>
-      <c r="BJ2" s="32" t="inlineStr">
-        <is>
-          <t>Chaîne de la valeur</t>
-        </is>
-      </c>
-      <c r="BK2" s="33"/>
-      <c r="BL2" s="33"/>
-      <c r="BM2" s="33"/>
-      <c r="BN2" s="33"/>
-      <c r="BO2" s="33"/>
-      <c r="BP2" s="33"/>
-      <c r="BQ2" s="33"/>
-      <c r="BR2" s="33"/>
-      <c r="BS2" s="34"/>
-      <c r="BT2" s="32" t="inlineStr">
-        <is>
-          <t>TRL</t>
-        </is>
-      </c>
-      <c r="BU2" s="34"/>
-      <c r="BV2" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="BW2" s="32" t="inlineStr">
-        <is>
-          <t>Feuille de route de WEAMEC (cocher)</t>
-        </is>
-      </c>
-      <c r="BX2" s="33"/>
-      <c r="BY2" s="33"/>
-      <c r="BZ2" s="33"/>
       <c r="CA2" s="33"/>
       <c r="CB2" s="33"/>
       <c r="CC2" s="33"/>
-      <c r="CD2" s="33"/>
-      <c r="CE2" s="33"/>
+      <c r="CD2" s="34"/>
+      <c r="CE2" s="32" t="inlineStr">
+        <is>
+          <t>Chaîne de la valeur</t>
+        </is>
+      </c>
       <c r="CF2" s="33"/>
       <c r="CG2" s="33"/>
       <c r="CH2" s="33"/>
-      <c r="CI2" s="34"/>
-      <c r="CJ2" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="CK2" s="36" t="inlineStr">
+      <c r="CI2" s="33"/>
+      <c r="CJ2" s="33"/>
+      <c r="CK2" s="33"/>
+      <c r="CL2" s="33"/>
+      <c r="CM2" s="33"/>
+      <c r="CN2" s="34"/>
+      <c r="CO2" s="32" t="inlineStr">
+        <is>
+          <t>TRL</t>
+        </is>
+      </c>
+      <c r="CP2" s="34"/>
+      <c r="CQ2" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="CR2" s="32" t="inlineStr">
+        <is>
+          <t>Feuille de route de WEAMEC (cocher)</t>
+        </is>
+      </c>
+      <c r="CS2" s="33"/>
+      <c r="CT2" s="33"/>
+      <c r="CU2" s="33"/>
+      <c r="CV2" s="33"/>
+      <c r="CW2" s="33"/>
+      <c r="CX2" s="33"/>
+      <c r="CY2" s="33"/>
+      <c r="CZ2" s="33"/>
+      <c r="DA2" s="33"/>
+      <c r="DB2" s="33"/>
+      <c r="DC2" s="33"/>
+      <c r="DD2" s="34"/>
+      <c r="DE2" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="DF2" s="36" t="inlineStr">
         <is>
           <t>Doctorat</t>
         </is>
       </c>
-      <c r="CL2" s="37" t="inlineStr">
+      <c r="DG2" s="37" t="inlineStr">
         <is>
           <t>Communication </t>
         </is>
       </c>
-      <c r="CM2" s="38"/>
-      <c r="CN2" s="38"/>
-      <c r="CO2" s="38"/>
-      <c r="CP2" s="38"/>
-      <c r="CQ2" s="38"/>
-      <c r="CR2" s="39"/>
-      <c r="CS2" s="38" t="inlineStr">
+      <c r="DH2" s="38"/>
+      <c r="DI2" s="38"/>
+      <c r="DJ2" s="38"/>
+      <c r="DK2" s="38"/>
+      <c r="DL2" s="38"/>
+      <c r="DM2" s="39"/>
+      <c r="DN2" s="38" t="inlineStr">
         <is>
           <t>Suites</t>
         </is>
       </c>
-      <c r="CT2" s="38"/>
-      <c r="CU2" s="38"/>
-      <c r="CV2" s="38"/>
-      <c r="CW2" s="39"/>
-      <c r="CX2" s="40"/>
+      <c r="DO2" s="38"/>
+      <c r="DP2" s="38"/>
+      <c r="DQ2" s="38"/>
+      <c r="DR2" s="39"/>
+      <c r="DS2" s="40"/>
     </row>
-    <row r="3" spans="1:102" customHeight="1" ht="95.4">
+    <row r="3" spans="1:123" customHeight="1" ht="95.4">
       <c r="A3" s="41" t="inlineStr">
         <is>
           <t>Nom du projet</t>
@@ -1015,437 +1133,500 @@
           <t>Porteur du projet : adresse mail </t>
         </is>
       </c>
-      <c r="P3" s="43" t="inlineStr">
-        <is>
-          <t>Partenaire 1 : Etalissement ou entreprise</t>
-        </is>
-      </c>
-      <c r="Q3" s="43" t="inlineStr">
-        <is>
-          <t>Partenaire 1 : code postal</t>
-        </is>
-      </c>
-      <c r="R3" s="43" t="inlineStr">
-        <is>
-          <t>Partenaire 1 : ville</t>
-        </is>
-      </c>
-      <c r="S3" s="43" t="inlineStr">
-        <is>
-          <t>Partenaire 1 : Laboratoire (si renseigné)</t>
-        </is>
-      </c>
-      <c r="T3" s="43" t="inlineStr">
-        <is>
-          <t>Partenaire 1 : Nom </t>
-        </is>
-      </c>
-      <c r="U3" s="43" t="inlineStr">
-        <is>
-          <t>Partenaire 1 : Prénom</t>
-        </is>
-      </c>
-      <c r="V3" s="43" t="inlineStr">
-        <is>
-          <t>Partenaire 1 : adresse mail</t>
-        </is>
-      </c>
-      <c r="W3" s="43" t="inlineStr">
-        <is>
-          <t>Partenaire 2 : Etalissement ou entreprise</t>
-        </is>
-      </c>
-      <c r="X3" s="43" t="inlineStr">
-        <is>
-          <t>Partenaire 2 : code postal</t>
-        </is>
-      </c>
-      <c r="Y3" s="43" t="inlineStr">
-        <is>
-          <t>Partenaire 2 : ville</t>
-        </is>
-      </c>
-      <c r="Z3" s="43" t="inlineStr">
-        <is>
-          <t>Partenaire 2 : Laboratoire (si renseigné)</t>
-        </is>
-      </c>
-      <c r="AA3" s="43" t="inlineStr">
-        <is>
-          <t>Partenaire 2 : Nom </t>
-        </is>
-      </c>
-      <c r="AB3" s="43" t="inlineStr">
-        <is>
-          <t>Partenaire 2 : Prénom</t>
-        </is>
-      </c>
-      <c r="AC3" s="43" t="inlineStr">
-        <is>
-          <t>Partenaire 2 : adresse mail</t>
-        </is>
-      </c>
-      <c r="AD3" s="43" t="inlineStr">
-        <is>
-          <t>Partenaire 3 : Etalissement ou entreprise</t>
-        </is>
-      </c>
-      <c r="AE3" s="43" t="inlineStr">
-        <is>
-          <t>Partenaire 3 : code postal</t>
-        </is>
-      </c>
-      <c r="AF3" s="43" t="inlineStr">
-        <is>
-          <t>Partenaire 3 : ville</t>
-        </is>
-      </c>
-      <c r="AG3" s="43" t="inlineStr">
-        <is>
-          <t>Partenaire 3 : Laboratoire (si renseigné)</t>
-        </is>
-      </c>
-      <c r="AH3" s="43" t="inlineStr">
-        <is>
-          <t>Partenaire 3 : Nom </t>
-        </is>
-      </c>
-      <c r="AI3" s="43" t="inlineStr">
-        <is>
-          <t>Partenaire 3 : Prénom</t>
-        </is>
-      </c>
-      <c r="AJ3" s="43" t="inlineStr">
-        <is>
-          <t>Partenaire 3 : adresse mail</t>
-        </is>
-      </c>
-      <c r="AK3" s="44" t="inlineStr">
+      <c r="P3" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="R3" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="S3" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="T3" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="U3" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="V3" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="W3" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="X3" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y3" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z3" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA3" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB3" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC3" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD3" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE3" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF3" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="AG3" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH3" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="AI3" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="AJ3" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="AK3" s="43" t="inlineStr">
+        <is>
+          <t>Partenaire 4 : Etalissement ou entreprise</t>
+        </is>
+      </c>
+      <c r="AL3" s="43" t="inlineStr">
+        <is>
+          <t>Partenaire 4 : code postal</t>
+        </is>
+      </c>
+      <c r="AM3" s="43" t="inlineStr">
+        <is>
+          <t>Partenaire 4 : ville</t>
+        </is>
+      </c>
+      <c r="AN3" s="43" t="inlineStr">
+        <is>
+          <t>Partenaire 4 : Laboratoire (si renseigné)</t>
+        </is>
+      </c>
+      <c r="AO3" s="43" t="inlineStr">
+        <is>
+          <t>Partenaire 4 : Nom </t>
+        </is>
+      </c>
+      <c r="AP3" s="43" t="inlineStr">
+        <is>
+          <t>Partenaire 4 : Prénom</t>
+        </is>
+      </c>
+      <c r="AQ3" s="43" t="inlineStr">
+        <is>
+          <t>Partenaire 4 : adresse mail</t>
+        </is>
+      </c>
+      <c r="AR3" s="43" t="inlineStr">
+        <is>
+          <t>Partenaire 5 : Etalissement ou entreprise</t>
+        </is>
+      </c>
+      <c r="AS3" s="43" t="inlineStr">
+        <is>
+          <t>Partenaire 5 : code postal</t>
+        </is>
+      </c>
+      <c r="AT3" s="43" t="inlineStr">
+        <is>
+          <t>Partenaire 5 : ville</t>
+        </is>
+      </c>
+      <c r="AU3" s="43" t="inlineStr">
+        <is>
+          <t>Partenaire 5 : Laboratoire (si renseigné)</t>
+        </is>
+      </c>
+      <c r="AV3" s="43" t="inlineStr">
+        <is>
+          <t>Partenaire 5 : Nom </t>
+        </is>
+      </c>
+      <c r="AW3" s="43" t="inlineStr">
+        <is>
+          <t>Partenaire 5 : Prénom</t>
+        </is>
+      </c>
+      <c r="AX3" s="43" t="inlineStr">
+        <is>
+          <t>Partenaire 5 : adresse mail</t>
+        </is>
+      </c>
+      <c r="AY3" s="43" t="inlineStr">
+        <is>
+          <t>Partenaire 6 : Etalissement ou entreprise</t>
+        </is>
+      </c>
+      <c r="AZ3" s="43" t="inlineStr">
+        <is>
+          <t>Partenaire 6 : code postal</t>
+        </is>
+      </c>
+      <c r="BA3" s="43" t="inlineStr">
+        <is>
+          <t>Partenaire 6 : ville</t>
+        </is>
+      </c>
+      <c r="BB3" s="43" t="inlineStr">
+        <is>
+          <t>Partenaire 6 : Laboratoire (si renseigné)</t>
+        </is>
+      </c>
+      <c r="BC3" s="43" t="inlineStr">
+        <is>
+          <t>Partenaire 6 : Nom </t>
+        </is>
+      </c>
+      <c r="BD3" s="43" t="inlineStr">
+        <is>
+          <t>Partenaire 6 : Prénom</t>
+        </is>
+      </c>
+      <c r="BE3" s="43" t="inlineStr">
+        <is>
+          <t>Partenaire 6 : adresse mail</t>
+        </is>
+      </c>
+      <c r="BF3" s="44" t="inlineStr">
         <is>
           <t>Coût total projet HT        (en €)</t>
         </is>
       </c>
-      <c r="AL3" s="44" t="inlineStr">
+      <c r="BG3" s="44" t="inlineStr">
         <is>
           <t>Montant financement WEAMEC (en €)</t>
         </is>
       </c>
-      <c r="AM3" s="44" t="inlineStr">
+      <c r="BH3" s="44" t="inlineStr">
         <is>
           <t>Dont PdL</t>
         </is>
       </c>
-      <c r="AN3" s="44" t="inlineStr">
+      <c r="BI3" s="44" t="inlineStr">
         <is>
           <t>Dont NM</t>
         </is>
       </c>
-      <c r="AO3" s="44" t="inlineStr">
+      <c r="BJ3" s="44" t="inlineStr">
         <is>
           <t>Dont CARENE</t>
         </is>
       </c>
-      <c r="AP3" s="44" t="inlineStr">
+      <c r="BK3" s="44" t="inlineStr">
         <is>
           <t>Dont FEDER</t>
         </is>
       </c>
-      <c r="AQ3" s="44" t="inlineStr">
+      <c r="BL3" s="44" t="inlineStr">
         <is>
           <t>Fonds propres</t>
         </is>
       </c>
-      <c r="AR3" s="44" t="inlineStr">
+      <c r="BM3" s="44" t="inlineStr">
         <is>
           <t>Cofinancement PdlL</t>
         </is>
       </c>
-      <c r="AS3" s="44" t="inlineStr">
+      <c r="BN3" s="44" t="inlineStr">
         <is>
           <t>Cofinancement CARENE</t>
         </is>
       </c>
-      <c r="AT3" s="44" t="inlineStr">
+      <c r="BO3" s="44" t="inlineStr">
         <is>
           <t>Cofinancement autre</t>
         </is>
       </c>
-      <c r="AU3" s="44" t="inlineStr">
+      <c r="BP3" s="44" t="inlineStr">
         <is>
           <t>Si autre cofinancement, préciser le nom du cofinanceur</t>
         </is>
       </c>
-      <c r="AV3" s="45" t="inlineStr">
+      <c r="BQ3" s="45" t="inlineStr">
         <is>
           <t>Nbre de doctorants</t>
         </is>
       </c>
-      <c r="AW3" s="46" t="inlineStr">
+      <c r="BR3" s="46" t="inlineStr">
         <is>
           <t>Nbre de mois de post-doc</t>
         </is>
       </c>
-      <c r="AX3" s="47" t="inlineStr">
+      <c r="BS3" s="47" t="inlineStr">
         <is>
           <t>1 Eolien posé</t>
         </is>
       </c>
-      <c r="AY3" s="47" t="inlineStr">
+      <c r="BT3" s="47" t="inlineStr">
         <is>
           <t>2 Eolien flottant</t>
         </is>
       </c>
-      <c r="AZ3" s="47" t="inlineStr">
+      <c r="BU3" s="47" t="inlineStr">
         <is>
           <t> 3 Hydrolien</t>
         </is>
       </c>
-      <c r="BA3" s="47" t="inlineStr">
+      <c r="BV3" s="47" t="inlineStr">
         <is>
           <t> 4 Houlomoteur</t>
         </is>
       </c>
-      <c r="BB3" s="47" t="inlineStr">
+      <c r="BW3" s="47" t="inlineStr">
         <is>
           <t>5 ETM</t>
         </is>
       </c>
-      <c r="BC3" s="47" t="inlineStr">
+      <c r="BX3" s="47" t="inlineStr">
         <is>
           <t>6 Osmotique</t>
         </is>
       </c>
-      <c r="BD3" s="47" t="inlineStr">
+      <c r="BY3" s="47" t="inlineStr">
         <is>
           <t>7 Solaire</t>
         </is>
       </c>
-      <c r="BE3" s="47" t="inlineStr">
+      <c r="BZ3" s="47" t="inlineStr">
         <is>
           <t> 1 Génie océanique</t>
         </is>
       </c>
-      <c r="BF3" s="47" t="inlineStr">
+      <c r="CA3" s="47" t="inlineStr">
         <is>
           <t> 2  Génie civil &amp; matériaux   </t>
         </is>
       </c>
-      <c r="BG3" s="47" t="inlineStr">
+      <c r="CB3" s="47" t="inlineStr">
         <is>
           <t>3 Génie électrique </t>
         </is>
       </c>
-      <c r="BH3" s="47" t="inlineStr">
+      <c r="CC3" s="47" t="inlineStr">
         <is>
           <t>4 Ressource et environnement naturel</t>
         </is>
       </c>
-      <c r="BI3" s="47" t="inlineStr">
+      <c r="CD3" s="47" t="inlineStr">
         <is>
           <t>5 Droit / Economie / Sécurité / Société    </t>
         </is>
       </c>
-      <c r="BJ3" s="48" t="inlineStr">
+      <c r="CE3" s="48" t="inlineStr">
         <is>
           <t>1 Caractérisation des sites et études environnementales</t>
         </is>
       </c>
-      <c r="BK3" s="48" t="inlineStr">
+      <c r="CF3" s="48" t="inlineStr">
         <is>
           <t>2 Ingénierie des parcs</t>
         </is>
       </c>
-      <c r="BL3" s="48" t="inlineStr">
+      <c r="CG3" s="48" t="inlineStr">
         <is>
           <t>3 Ingénierie des machines / du réseau énergétique</t>
         </is>
       </c>
-      <c r="BM3" s="48" t="inlineStr">
+      <c r="CH3" s="48" t="inlineStr">
         <is>
           <t>4 Ingénierie de fabrication / transport / installation</t>
         </is>
       </c>
-      <c r="BN3" s="48" t="inlineStr">
+      <c r="CI3" s="48" t="inlineStr">
         <is>
           <t>5 Fabrication</t>
         </is>
       </c>
-      <c r="BO3" s="48" t="inlineStr">
+      <c r="CJ3" s="48" t="inlineStr">
         <is>
           <t>6 Installation en mer / Certification / Mise en service</t>
         </is>
       </c>
-      <c r="BP3" s="48" t="inlineStr">
+      <c r="CK3" s="48" t="inlineStr">
         <is>
           <t>7 Exploitation / Maintenance / SHM</t>
         </is>
       </c>
-      <c r="BQ3" s="48" t="inlineStr">
+      <c r="CL3" s="48" t="inlineStr">
         <is>
           <t>8 Sécurité / Sûreté</t>
         </is>
       </c>
-      <c r="BR3" s="48" t="inlineStr">
+      <c r="CM3" s="48" t="inlineStr">
         <is>
           <t>9 Démantèlement et Recyclage</t>
         </is>
       </c>
-      <c r="BS3" s="48" t="inlineStr">
+      <c r="CN3" s="48" t="inlineStr">
         <is>
           <t>10 Services support</t>
         </is>
       </c>
-      <c r="BT3" s="47" t="inlineStr">
+      <c r="CO3" s="47" t="inlineStr">
         <is>
           <t>TRL début</t>
         </is>
       </c>
-      <c r="BU3" s="47" t="inlineStr">
+      <c r="CP3" s="47" t="inlineStr">
         <is>
           <t>TRL fin</t>
         </is>
       </c>
-      <c r="BV3" s="47" t="inlineStr">
+      <c r="CQ3" s="47" t="inlineStr">
         <is>
           <t>Brevet visé?</t>
         </is>
       </c>
-      <c r="BW3" s="47" t="inlineStr">
+      <c r="CR3" s="47" t="inlineStr">
         <is>
           <t>Priorité 1</t>
         </is>
       </c>
-      <c r="BX3" s="47" t="inlineStr">
+      <c r="CS3" s="47" t="inlineStr">
         <is>
           <t>Priorité 2</t>
         </is>
       </c>
-      <c r="BY3" s="47" t="inlineStr">
+      <c r="CT3" s="47" t="inlineStr">
         <is>
           <t>Objectif 1</t>
         </is>
       </c>
-      <c r="BZ3" s="47" t="inlineStr">
+      <c r="CU3" s="47" t="inlineStr">
         <is>
           <t>Objectif 2</t>
         </is>
       </c>
-      <c r="CA3" s="47" t="inlineStr">
+      <c r="CV3" s="47" t="inlineStr">
         <is>
           <t>Objectif 3</t>
         </is>
       </c>
-      <c r="CB3" s="47" t="inlineStr">
+      <c r="CW3" s="47" t="inlineStr">
         <is>
           <t>Objectif 4</t>
         </is>
       </c>
-      <c r="CC3" s="47" t="inlineStr">
+      <c r="CX3" s="47" t="inlineStr">
         <is>
           <t>Défi 1</t>
         </is>
       </c>
-      <c r="CD3" s="47" t="inlineStr">
+      <c r="CY3" s="47" t="inlineStr">
         <is>
           <t>Défi 2</t>
         </is>
       </c>
-      <c r="CE3" s="47" t="inlineStr">
+      <c r="CZ3" s="47" t="inlineStr">
         <is>
           <t>Défi 3</t>
         </is>
       </c>
-      <c r="CF3" s="47" t="inlineStr">
+      <c r="DA3" s="47" t="inlineStr">
         <is>
           <t>Défi 4</t>
         </is>
       </c>
-      <c r="CG3" s="47" t="inlineStr">
+      <c r="DB3" s="47" t="inlineStr">
         <is>
           <t>Défi 5</t>
         </is>
       </c>
-      <c r="CH3" s="47" t="inlineStr">
+      <c r="DC3" s="47" t="inlineStr">
         <is>
           <t>Défi 6</t>
         </is>
       </c>
-      <c r="CI3" s="47" t="inlineStr">
+      <c r="DD3" s="47" t="inlineStr">
         <is>
           <t>Défi 7</t>
         </is>
       </c>
-      <c r="CJ3" s="49" t="inlineStr">
+      <c r="DE3" s="49" t="inlineStr">
         <is>
           <t>Brevet déposé?</t>
         </is>
       </c>
-      <c r="CK3" s="49" t="inlineStr">
+      <c r="DF3" s="49" t="inlineStr">
         <is>
           <t>Si thèse, date de la soutenance</t>
         </is>
       </c>
-      <c r="CL3" s="49" t="inlineStr">
+      <c r="DG3" s="49" t="inlineStr">
         <is>
           <t>Articles publiés</t>
         </is>
       </c>
-      <c r="CM3" s="49" t="inlineStr">
+      <c r="DH3" s="49" t="inlineStr">
         <is>
           <t>Participations congrès Actes à comité de lecture</t>
         </is>
       </c>
-      <c r="CN3" s="49" t="inlineStr">
+      <c r="DI3" s="49" t="inlineStr">
         <is>
           <t>Participations congrès Actes à diffusion restreinte</t>
         </is>
       </c>
-      <c r="CO3" s="49" t="inlineStr">
+      <c r="DJ3" s="49" t="inlineStr">
         <is>
           <t>Publication de données en open source</t>
         </is>
       </c>
-      <c r="CP3" s="49" t="inlineStr">
+      <c r="DK3" s="49" t="inlineStr">
         <is>
           <t>actions de formation</t>
         </is>
       </c>
-      <c r="CQ3" s="49" t="inlineStr">
+      <c r="DL3" s="49" t="inlineStr">
         <is>
           <t>webinaire</t>
         </is>
       </c>
-      <c r="CR3" s="49" t="inlineStr">
+      <c r="DM3" s="49" t="inlineStr">
         <is>
           <t>Vulgarisation scientifique</t>
         </is>
       </c>
-      <c r="CS3" s="49" t="inlineStr">
+      <c r="DN3" s="49" t="inlineStr">
         <is>
           <t>Permet l'aboutissement d'un autre projet?</t>
         </is>
       </c>
-      <c r="CT3" s="49" t="inlineStr">
+      <c r="DO3" s="49" t="inlineStr">
         <is>
           <t>Budget de cet autre projet</t>
         </is>
       </c>
-      <c r="CU3" s="49" t="inlineStr">
+      <c r="DP3" s="49" t="inlineStr">
         <is>
           <t>Source financement (envisagée)</t>
         </is>
       </c>
-      <c r="CV3" s="49" t="inlineStr">
+      <c r="DQ3" s="49" t="inlineStr">
         <is>
           <t>Collaborations issues du projet</t>
         </is>
       </c>
-      <c r="CW3" s="49" t="inlineStr">
+      <c r="DR3" s="49" t="inlineStr">
         <is>
           <t>Apport aux entreprises : brevet vendu ou implication financière?</t>
         </is>
       </c>
-      <c r="CX3" s="50" t="inlineStr">
+      <c r="DS3" s="50" t="inlineStr">
         <is>
           <t>Projet terminé (cocher)</t>
         </is>
@@ -1460,20 +1641,23 @@
     <mergeCell ref="P2:V2"/>
     <mergeCell ref="W2:AC2"/>
     <mergeCell ref="AD2:AJ2"/>
-    <mergeCell ref="AK2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:BD2"/>
-    <mergeCell ref="BE2:BI2"/>
-    <mergeCell ref="BJ2:BS2"/>
-    <mergeCell ref="BT2:BU2"/>
-    <mergeCell ref="BW2:CI2"/>
-    <mergeCell ref="CL2:CR2"/>
-    <mergeCell ref="CS2:CW2"/>
+    <mergeCell ref="AK2:AQ2"/>
+    <mergeCell ref="AR2:AX2"/>
+    <mergeCell ref="AY2:BE2"/>
+    <mergeCell ref="BF2:BP2"/>
+    <mergeCell ref="BQ2:BR2"/>
+    <mergeCell ref="BS2:BY2"/>
+    <mergeCell ref="BZ2:CD2"/>
+    <mergeCell ref="CE2:CN2"/>
+    <mergeCell ref="CO2:CP2"/>
+    <mergeCell ref="CR2:DD2"/>
+    <mergeCell ref="DG2:DM2"/>
+    <mergeCell ref="DN2:DR2"/>
     <mergeCell ref="B1:I1"/>
-    <mergeCell ref="J1:AJ1"/>
-    <mergeCell ref="AK1:AW1"/>
-    <mergeCell ref="AX1:CI1"/>
-    <mergeCell ref="CJ1:CW1"/>
+    <mergeCell ref="J1:BE1"/>
+    <mergeCell ref="BF1:BR1"/>
+    <mergeCell ref="BS1:DD1"/>
+    <mergeCell ref="DE1:DR1"/>
   </mergeCells>
   <printOptions/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1492,7 +1676,7 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -1502,8 +1686,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" customHeight="1" ht="19.5">
-      <c r="A1" s="51" t="s">
-        <v>1</v>
+      <c r="A1" s="51" t="inlineStr">
+        <is>
+          <t>EXPERTS</t>
+        </is>
       </c>
       <c r="B1" s="51"/>
       <c r="C1" s="51"/>

</xml_diff>